<commit_message>
patient file & some front end stuff
</commit_message>
<xml_diff>
--- a/Database Model.xlsx
+++ b/Database Model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KingSameulX/Desktop/Xcode/2020_05/P2P/v2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KingSameulX/Desktop/Xcode/2020_05/P2P/v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D928D9-3218-7546-A914-BF95C10A00B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4F39DC-8BCA-0847-8302-DEC580159CC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{EDB24821-F2C5-425D-B33E-6AD2066199ED}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
   <si>
     <t>Username</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>postInfoP</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>patientlist</t>
   </si>
 </sst>
 </file>
@@ -219,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -372,11 +378,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -430,79 +449,97 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -819,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3988128D-3FD2-47DC-9839-E9F293FB2200}">
-  <dimension ref="A1:W29"/>
+  <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -831,22 +868,27 @@
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" customWidth="1"/>
-    <col min="15" max="15" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.5" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="10.1640625" customWidth="1"/>
+    <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="3"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -855,8 +897,11 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>24</v>
@@ -867,19 +912,22 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="43" t="s">
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="45" t="s">
+      <c r="D4" s="25"/>
+      <c r="E4" s="21" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -888,54 +936,63 @@
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C5" s="21" t="s">
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C6" s="21" t="s">
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C6" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C7" s="21" t="s">
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C7" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
@@ -951,12 +1008,15 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C8" s="21" t="s">
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="C8" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="34"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="7" t="s">
         <v>9</v>
       </c>
@@ -972,22 +1032,27 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
-    </row>
-    <row r="9" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="41" t="s">
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+    </row>
+    <row r="9" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="42"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="J9" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
@@ -995,102 +1060,133 @@
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
-    </row>
-    <row r="10" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="25" t="s">
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+    </row>
+    <row r="10" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="40"/>
+      <c r="D10" s="33"/>
       <c r="E10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="26"/>
-      <c r="I10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="34"/>
+      <c r="L10" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+    </row>
+    <row r="12" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="28"/>
-      <c r="I12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="29"/>
+      <c r="L12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
-    </row>
-    <row r="13" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+    </row>
+    <row r="13" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="6"/>
+      <c r="J13" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="39"/>
-      <c r="I13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="38" t="s">
+      <c r="K13" s="31"/>
+      <c r="L13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="N13" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="39"/>
-      <c r="M13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="14" t="s">
+        <v>9</v>
+      </c>
       <c r="Q13" s="6"/>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1099,19 +1195,22 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="21" t="s">
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="L14" s="22"/>
-      <c r="M14" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="Q14" s="6"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1120,19 +1219,22 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="21" t="s">
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
+      <c r="O15" s="35"/>
+      <c r="P15" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="Q15" s="6"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1141,19 +1243,22 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="21" t="s">
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="L16" s="22"/>
-      <c r="M16" s="15" t="s">
+      <c r="O16" s="35"/>
+      <c r="P16" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1162,19 +1267,22 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="21" t="s">
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="L17" s="22"/>
-      <c r="M17" s="15" t="s">
+      <c r="O17" s="35"/>
+      <c r="P17" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
-    </row>
-    <row r="18" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+    </row>
+    <row r="18" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1183,21 +1291,24 @@
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="21" t="s">
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="L18" s="22"/>
-      <c r="M18" s="15" t="s">
+      <c r="O18" s="35"/>
+      <c r="P18" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6" t="s">
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-    </row>
-    <row r="19" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+    </row>
+    <row r="19" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1206,23 +1317,26 @@
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
-      <c r="K19" s="32" t="s">
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="L19" s="35"/>
-      <c r="M19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="N19" s="6"/>
-      <c r="O19" s="32" t="s">
+      <c r="O19" s="37"/>
+      <c r="P19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="S19" s="37"/>
+      <c r="T19" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -1235,15 +1349,18 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
-      <c r="O20" s="36" t="s">
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="15" t="s">
+      <c r="S20" s="39"/>
+      <c r="T20" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -1256,15 +1373,18 @@
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
-      <c r="O21" s="23" t="s">
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S21" s="41"/>
+      <c r="T21" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="20"/>
@@ -1282,133 +1402,151 @@
       <c r="O22" s="20"/>
       <c r="P22" s="20"/>
       <c r="Q22" s="20"/>
-      <c r="R22" s="19"/>
-      <c r="S22" s="19"/>
-      <c r="T22" s="19"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="20"/>
       <c r="U22" s="19"/>
       <c r="V22" s="19"/>
       <c r="W22" s="19"/>
-    </row>
-    <row r="23" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X22" s="19"/>
+      <c r="Y22" s="19"/>
+      <c r="Z22" s="19"/>
+    </row>
+    <row r="23" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
+      <c r="J23" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
-      <c r="O23" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
-    </row>
-    <row r="24" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+    </row>
+    <row r="24" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="26"/>
-      <c r="I24" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="6"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
-      <c r="O24" s="32" t="s">
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="S24" s="45"/>
+      <c r="T24" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H25" s="28"/>
-      <c r="I25" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
-      <c r="O25" s="21" t="s">
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S25" s="27"/>
+      <c r="T25" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-      <c r="G26" s="29" t="s">
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="H26" s="30"/>
-      <c r="I26" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="6"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
-      <c r="O26" s="21" t="s">
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="15" t="s">
+      <c r="S26" s="35"/>
+      <c r="T26" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-      <c r="G27" s="23" t="s">
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="31"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="6"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="6"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="17"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
-      <c r="O27" s="21" t="s">
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="15" t="s">
+      <c r="S27" s="35"/>
+      <c r="T27" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1421,52 +1559,55 @@
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
-      <c r="O28" s="21" t="s">
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="15" t="s">
+      <c r="S28" s="35"/>
+      <c r="T28" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="O29" s="23"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="4"/>
+    <row r="29" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R29" s="40"/>
+      <c r="S29" s="42"/>
+      <c r="T29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="R28:S28"/>
+    <mergeCell ref="R29:S29"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="R24:S24"/>
+    <mergeCell ref="R25:S25"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="O27:P27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new patient route nesting
</commit_message>
<xml_diff>
--- a/Database Model.xlsx
+++ b/Database Model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KingSameulX/Desktop/Xcode/2020_05/P2P/v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4F39DC-8BCA-0847-8302-DEC580159CC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9EAA03-22EE-B84D-A031-8DED35F7BF93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{EDB24821-F2C5-425D-B33E-6AD2066199ED}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" xr2:uid="{EDB24821-F2C5-425D-B33E-6AD2066199ED}"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>
@@ -146,9 +146,6 @@
     <t>docReg</t>
   </si>
   <si>
-    <t>patInfo</t>
-  </si>
-  <si>
     <t>diagInfo</t>
   </si>
   <si>
@@ -164,7 +161,10 @@
     <t>username</t>
   </si>
   <si>
-    <t>patientlist</t>
+    <t>doc_pat_list</t>
+  </si>
+  <si>
+    <t>pat_Info</t>
   </si>
 </sst>
 </file>
@@ -452,6 +452,84 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -463,84 +541,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -859,7 +859,7 @@
   <dimension ref="A1:Z29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -917,10 +917,10 @@
       <c r="L3" s="2"/>
     </row>
     <row r="4" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="51"/>
       <c r="E4" s="21" t="s">
         <v>9</v>
       </c>
@@ -941,10 +941,10 @@
       <c r="T4" s="6"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="41"/>
       <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
@@ -965,10 +965,10 @@
       <c r="T5" s="6"/>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="27"/>
+      <c r="D6" s="41"/>
       <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
@@ -989,10 +989,10 @@
       <c r="T6" s="6"/>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="27"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1013,10 +1013,10 @@
       <c r="T7" s="6"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="27"/>
+      <c r="D8" s="41"/>
       <c r="E8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1037,21 +1037,21 @@
       <c r="T8" s="6"/>
     </row>
     <row r="9" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="49"/>
       <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -1068,22 +1068,22 @@
       <c r="C10" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="47"/>
       <c r="E10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="49" t="s">
+      <c r="G10" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="25" t="s">
         <v>7</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="34"/>
+      <c r="K10" s="33"/>
       <c r="L10" s="11" t="s">
         <v>9</v>
       </c>
@@ -1101,17 +1101,17 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="50" t="s">
+      <c r="G11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="26" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="6"/>
-      <c r="J11" s="28" t="s">
+      <c r="J11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="K11" s="29"/>
+      <c r="K11" s="35"/>
       <c r="L11" s="12" t="s">
         <v>9</v>
       </c>
@@ -1129,23 +1129,23 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="50" t="s">
+      <c r="G12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H12" s="26" t="s">
         <v>7</v>
       </c>
       <c r="I12" s="6"/>
-      <c r="J12" s="28" t="s">
+      <c r="J12" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="29"/>
+      <c r="K12" s="35"/>
       <c r="L12" s="12" t="s">
         <v>9</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
@@ -1159,25 +1159,25 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" s="51" t="s">
+      <c r="G13" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="27" t="s">
         <v>7</v>
       </c>
       <c r="I13" s="6"/>
-      <c r="J13" s="30" t="s">
+      <c r="J13" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="31"/>
+      <c r="K13" s="46"/>
       <c r="L13" s="13" t="s">
         <v>9</v>
       </c>
       <c r="M13" s="6"/>
-      <c r="N13" s="30" t="s">
+      <c r="N13" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="31"/>
+      <c r="O13" s="46"/>
       <c r="P13" s="14" t="s">
         <v>9</v>
       </c>
@@ -1198,10 +1198,10 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="26" t="s">
+      <c r="N14" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="O14" s="35"/>
+      <c r="O14" s="29"/>
       <c r="P14" s="15" t="s">
         <v>9</v>
       </c>
@@ -1222,10 +1222,10 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="26" t="s">
+      <c r="N15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="35"/>
+      <c r="O15" s="29"/>
       <c r="P15" s="15" t="s">
         <v>9</v>
       </c>
@@ -1246,10 +1246,10 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="26" t="s">
+      <c r="N16" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="O16" s="35"/>
+      <c r="O16" s="29"/>
       <c r="P16" s="15" t="s">
         <v>10</v>
       </c>
@@ -1270,10 +1270,10 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="26" t="s">
+      <c r="N17" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="O17" s="35"/>
+      <c r="O17" s="29"/>
       <c r="P17" s="15" t="s">
         <v>10</v>
       </c>
@@ -1294,16 +1294,16 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="26" t="s">
+      <c r="N18" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="O18" s="35"/>
+      <c r="O18" s="29"/>
       <c r="P18" s="15" t="s">
         <v>10</v>
       </c>
       <c r="Q18" s="6"/>
       <c r="R18" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
@@ -1320,18 +1320,18 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-      <c r="N19" s="36" t="s">
+      <c r="N19" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="O19" s="37"/>
+      <c r="O19" s="42"/>
       <c r="P19" s="16" t="s">
         <v>9</v>
       </c>
       <c r="Q19" s="6"/>
-      <c r="R19" s="36" t="s">
+      <c r="R19" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="S19" s="37"/>
+      <c r="S19" s="42"/>
       <c r="T19" s="16" t="s">
         <v>9</v>
       </c>
@@ -1352,10 +1352,10 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
-      <c r="R20" s="38" t="s">
+      <c r="R20" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="S20" s="39"/>
+      <c r="S20" s="44"/>
       <c r="T20" s="15" t="s">
         <v>10</v>
       </c>
@@ -1376,10 +1376,10 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="40" t="s">
+      <c r="R21" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="S21" s="41"/>
+      <c r="S21" s="38"/>
       <c r="T21" s="17" t="s">
         <v>9</v>
       </c>
@@ -1421,7 +1421,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
@@ -1431,7 +1431,7 @@
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
@@ -1447,7 +1447,7 @@
       <c r="J24" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K24" s="34"/>
+      <c r="K24" s="33"/>
       <c r="L24" s="11" t="s">
         <v>9</v>
       </c>
@@ -1456,10 +1456,10 @@
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
-      <c r="R24" s="36" t="s">
+      <c r="R24" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="S24" s="45"/>
+      <c r="S24" s="40"/>
       <c r="T24" s="16" t="s">
         <v>9</v>
       </c>
@@ -1472,10 +1472,10 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="28" t="s">
+      <c r="J25" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="K25" s="29"/>
+      <c r="K25" s="35"/>
       <c r="L25" s="12" t="s">
         <v>9</v>
       </c>
@@ -1484,10 +1484,10 @@
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
-      <c r="R25" s="26" t="s">
+      <c r="R25" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="S25" s="27"/>
+      <c r="S25" s="41"/>
       <c r="T25" s="15" t="s">
         <v>9</v>
       </c>
@@ -1500,10 +1500,10 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="43" t="s">
+      <c r="J26" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="44"/>
+      <c r="K26" s="37"/>
       <c r="L26" s="18" t="s">
         <v>9</v>
       </c>
@@ -1512,10 +1512,10 @@
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
-      <c r="R26" s="26" t="s">
+      <c r="R26" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="S26" s="35"/>
+      <c r="S26" s="29"/>
       <c r="T26" s="15" t="s">
         <v>10</v>
       </c>
@@ -1528,20 +1528,20 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
-      <c r="J27" s="40" t="s">
+      <c r="J27" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="K27" s="41"/>
+      <c r="K27" s="38"/>
       <c r="L27" s="17"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
-      <c r="R27" s="26" t="s">
+      <c r="R27" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="S27" s="35"/>
+      <c r="S27" s="29"/>
       <c r="T27" s="15" t="s">
         <v>10</v>
       </c>
@@ -1562,21 +1562,42 @@
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
-      <c r="R28" s="26" t="s">
+      <c r="R28" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="S28" s="35"/>
+      <c r="S28" s="29"/>
       <c r="T28" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R29" s="40"/>
-      <c r="S29" s="42"/>
+      <c r="R29" s="30"/>
+      <c r="S29" s="31"/>
       <c r="T29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="R19:S19"/>
+    <mergeCell ref="R20:S20"/>
+    <mergeCell ref="R21:S21"/>
     <mergeCell ref="R28:S28"/>
     <mergeCell ref="R29:S29"/>
     <mergeCell ref="J24:K24"/>
@@ -1587,27 +1608,6 @@
     <mergeCell ref="R25:S25"/>
     <mergeCell ref="R26:S26"/>
     <mergeCell ref="R27:S27"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
backup for database redesign
</commit_message>
<xml_diff>
--- a/Database Model.xlsx
+++ b/Database Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KingSameulX/Desktop/Xcode/2020_05/P2P/v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9EAA03-22EE-B84D-A031-8DED35F7BF93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC98D685-AD68-1E48-B8FA-D9A13CF2E5E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" xr2:uid="{EDB24821-F2C5-425D-B33E-6AD2066199ED}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{EDB24821-F2C5-425D-B33E-6AD2066199ED}"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -541,6 +541,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -856,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3988128D-3FD2-47DC-9839-E9F293FB2200}">
-  <dimension ref="A1:Z29"/>
+  <dimension ref="A1:AA29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -869,13 +878,14 @@
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.5" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" customWidth="1"/>
-    <col min="11" max="11" width="10.1640625" customWidth="1"/>
-    <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" customWidth="1"/>
+    <col min="9" max="10" width="9.5" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" customWidth="1"/>
+    <col min="19" max="19" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -884,11 +894,12 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="1"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="2"/>
       <c r="L1" s="1"/>
-    </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -900,8 +911,9 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>24</v>
@@ -915,8 +927,9 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C4" s="50" t="s">
         <v>0</v>
       </c>
@@ -928,7 +941,7 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="6"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
@@ -939,8 +952,9 @@
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U4" s="6"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C5" s="28" t="s">
         <v>1</v>
       </c>
@@ -952,10 +966,10 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
+      <c r="J5" s="6"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
-      <c r="M5" s="6"/>
+      <c r="M5" s="8"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
@@ -963,8 +977,9 @@
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
-    </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U5" s="6"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C6" s="28" t="s">
         <v>2</v>
       </c>
@@ -976,10 +991,10 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="8"/>
+      <c r="J6" s="6"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
-      <c r="M6" s="6"/>
+      <c r="M6" s="8"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
@@ -987,8 +1002,9 @@
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
-    </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U6" s="6"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C7" s="28" t="s">
         <v>3</v>
       </c>
@@ -1011,8 +1027,9 @@
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U7" s="6"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C8" s="28" t="s">
         <v>6</v>
       </c>
@@ -1035,8 +1052,9 @@
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
-    </row>
-    <row r="9" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U8" s="6"/>
+    </row>
+    <row r="9" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="48" t="s">
         <v>8</v>
       </c>
@@ -1050,10 +1068,10 @@
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="6"/>
+      <c r="K9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
@@ -1063,8 +1081,9 @@
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
-    </row>
-    <row r="10" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U9" s="6"/>
+    </row>
+    <row r="10" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C10" s="32" t="s">
         <v>11</v>
       </c>
@@ -1076,18 +1095,18 @@
       <c r="G10" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="52"/>
+      <c r="I10" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="6"/>
+      <c r="K10" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="33"/>
-      <c r="L10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="M10" s="6"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
@@ -1095,8 +1114,9 @@
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U10" s="6"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1104,18 +1124,18 @@
       <c r="G11" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="53"/>
+      <c r="I11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="6"/>
+      <c r="K11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="K11" s="35"/>
-      <c r="L11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" s="6"/>
+      <c r="L11" s="35"/>
+      <c r="M11" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
@@ -1123,8 +1143,9 @@
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
-    </row>
-    <row r="12" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="6"/>
+    </row>
+    <row r="12" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1132,29 +1153,30 @@
       <c r="G12" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="53"/>
+      <c r="I12" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="34" t="s">
+      <c r="J12" s="6"/>
+      <c r="K12" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="35"/>
-      <c r="L12" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6" t="s">
+      <c r="L12" s="35"/>
+      <c r="M12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
-    </row>
-    <row r="13" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U12" s="6"/>
+    </row>
+    <row r="13" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1162,31 +1184,32 @@
       <c r="G13" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="54"/>
+      <c r="I13" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="45" t="s">
+      <c r="J13" s="6"/>
+      <c r="K13" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="46"/>
-      <c r="L13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="45" t="s">
+      <c r="L13" s="46"/>
+      <c r="M13" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="46"/>
-      <c r="P13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q13" s="6"/>
+      <c r="P13" s="46"/>
+      <c r="Q13" s="14" t="s">
+        <v>9</v>
+      </c>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U13" s="6"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1198,19 +1221,20 @@
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
-      <c r="N14" s="28" t="s">
+      <c r="N14" s="6"/>
+      <c r="O14" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="O14" s="29"/>
-      <c r="P14" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q14" s="6"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U14" s="6"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1222,19 +1246,20 @@
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
-      <c r="N15" s="28" t="s">
+      <c r="N15" s="6"/>
+      <c r="O15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="O15" s="29"/>
-      <c r="P15" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q15" s="6"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="15" t="s">
+        <v>9</v>
+      </c>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="U15" s="6"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1246,19 +1271,20 @@
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
-      <c r="N16" s="28" t="s">
+      <c r="N16" s="6"/>
+      <c r="O16" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="O16" s="29"/>
-      <c r="P16" s="15" t="s">
+      <c r="P16" s="29"/>
+      <c r="Q16" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="U16" s="6"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1270,19 +1296,20 @@
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
-      <c r="N17" s="28" t="s">
+      <c r="N17" s="6"/>
+      <c r="O17" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="O17" s="29"/>
-      <c r="P17" s="15" t="s">
+      <c r="P17" s="29"/>
+      <c r="Q17" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
-    </row>
-    <row r="18" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U17" s="6"/>
+    </row>
+    <row r="18" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1294,21 +1321,22 @@
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="28" t="s">
+      <c r="N18" s="6"/>
+      <c r="O18" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="O18" s="29"/>
-      <c r="P18" s="15" t="s">
+      <c r="P18" s="29"/>
+      <c r="Q18" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6" t="s">
+      <c r="R18" s="6"/>
+      <c r="S18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="S18" s="6"/>
       <c r="T18" s="6"/>
-    </row>
-    <row r="19" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U18" s="6"/>
+    </row>
+    <row r="19" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1320,23 +1348,24 @@
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-      <c r="N19" s="39" t="s">
+      <c r="N19" s="6"/>
+      <c r="O19" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="O19" s="42"/>
-      <c r="P19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="39" t="s">
+      <c r="P19" s="42"/>
+      <c r="Q19" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="R19" s="6"/>
+      <c r="S19" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="S19" s="42"/>
-      <c r="T19" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="T19" s="42"/>
+      <c r="U19" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -1352,15 +1381,16 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
-      <c r="R20" s="43" t="s">
+      <c r="R20" s="6"/>
+      <c r="S20" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="S20" s="44"/>
-      <c r="T20" s="15" t="s">
+      <c r="T20" s="44"/>
+      <c r="U20" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -1376,15 +1406,16 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
-      <c r="R21" s="30" t="s">
+      <c r="R21" s="6"/>
+      <c r="S21" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="S21" s="38"/>
-      <c r="T21" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T21" s="38"/>
+      <c r="U21" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="20"/>
@@ -1405,14 +1436,15 @@
       <c r="R22" s="20"/>
       <c r="S22" s="20"/>
       <c r="T22" s="20"/>
-      <c r="U22" s="19"/>
+      <c r="U22" s="20"/>
       <c r="V22" s="19"/>
       <c r="W22" s="19"/>
       <c r="X22" s="19"/>
       <c r="Y22" s="19"/>
       <c r="Z22" s="19"/>
-    </row>
-    <row r="23" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AA22" s="19"/>
+    </row>
+    <row r="23" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1420,23 +1452,24 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
-      <c r="J23" s="6" t="s">
+      <c r="J23" s="6"/>
+      <c r="K23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K23" s="6"/>
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
-      <c r="R23" s="6" t="s">
+      <c r="R23" s="6"/>
+      <c r="S23" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="S23" s="6"/>
       <c r="T23" s="6"/>
-    </row>
-    <row r="24" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="U23" s="6"/>
+    </row>
+    <row r="24" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1444,27 +1477,28 @@
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="32" t="s">
+      <c r="J24" s="6"/>
+      <c r="K24" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K24" s="33"/>
-      <c r="L24" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="M24" s="6"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
-      <c r="R24" s="39" t="s">
+      <c r="R24" s="6"/>
+      <c r="S24" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="S24" s="40"/>
-      <c r="T24" s="16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="T24" s="40"/>
+      <c r="U24" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -1472,27 +1506,28 @@
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
-      <c r="J25" s="34" t="s">
+      <c r="J25" s="6"/>
+      <c r="K25" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="K25" s="35"/>
-      <c r="L25" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="M25" s="6"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
-      <c r="R25" s="28" t="s">
+      <c r="R25" s="6"/>
+      <c r="S25" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="S25" s="41"/>
-      <c r="T25" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="T25" s="41"/>
+      <c r="U25" s="15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
@@ -1500,27 +1535,28 @@
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="36" t="s">
+      <c r="J26" s="6"/>
+      <c r="K26" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="37"/>
-      <c r="L26" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="M26" s="6"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="18" t="s">
+        <v>9</v>
+      </c>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
-      <c r="R26" s="28" t="s">
+      <c r="R26" s="6"/>
+      <c r="S26" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="S26" s="29"/>
-      <c r="T26" s="15" t="s">
+      <c r="T26" s="29"/>
+      <c r="U26" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -1528,25 +1564,26 @@
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
-      <c r="J27" s="30" t="s">
+      <c r="J27" s="6"/>
+      <c r="K27" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="K27" s="38"/>
-      <c r="L27" s="17"/>
-      <c r="M27" s="6"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="17"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
-      <c r="R27" s="28" t="s">
+      <c r="R27" s="6"/>
+      <c r="S27" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="S27" s="29"/>
-      <c r="T27" s="15" t="s">
+      <c r="T27" s="29"/>
+      <c r="U27" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
@@ -1562,18 +1599,19 @@
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
-      <c r="R28" s="28" t="s">
+      <c r="R28" s="6"/>
+      <c r="S28" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="S28" s="29"/>
-      <c r="T28" s="15" t="s">
+      <c r="T28" s="29"/>
+      <c r="U28" s="15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="R29" s="30"/>
-      <c r="S29" s="31"/>
-      <c r="T29" s="4"/>
+    <row r="29" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S29" s="30"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -1583,31 +1621,31 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="R19:S19"/>
-    <mergeCell ref="R20:S20"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="R28:S28"/>
-    <mergeCell ref="R29:S29"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="R24:S24"/>
-    <mergeCell ref="R25:S25"/>
-    <mergeCell ref="R26:S26"/>
-    <mergeCell ref="R27:S27"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="S28:T28"/>
+    <mergeCell ref="S29:T29"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="S27:T27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Front End housing keeping login
</commit_message>
<xml_diff>
--- a/Database Model.xlsx
+++ b/Database Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KingSameulX/Desktop/Xcode/2020_05/P2P/v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EA01BA-5C4F-8E44-9EC8-B681663CA44D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E69824F-F69B-E445-894D-3F6070FDBD53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{EDB24821-F2C5-425D-B33E-6AD2066199ED}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" xr2:uid="{EDB24821-F2C5-425D-B33E-6AD2066199ED}"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>
@@ -470,119 +470,119 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -963,10 +963,10 @@
       <c r="M3" s="2"/>
     </row>
     <row r="4" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="50"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="20" t="s">
         <v>9</v>
       </c>
@@ -988,10 +988,10 @@
       <c r="U4" s="6"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
@@ -1013,10 +1013,10 @@
       <c r="U5" s="6"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="40"/>
+      <c r="D6" s="42"/>
       <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1038,10 +1038,10 @@
       <c r="U6" s="6"/>
     </row>
     <row r="7" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="40"/>
+      <c r="D7" s="42"/>
       <c r="E7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1065,10 +1065,10 @@
       <c r="U7" s="6"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="40"/>
+      <c r="D8" s="42"/>
       <c r="E8" s="7" t="s">
         <v>9</v>
       </c>
@@ -1077,11 +1077,11 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="54" t="s">
+      <c r="K8" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="L8" s="55"/>
-      <c r="M8" s="63" t="s">
+      <c r="L8" s="36"/>
+      <c r="M8" s="31" t="s">
         <v>10</v>
       </c>
       <c r="N8" s="6"/>
@@ -1094,10 +1094,10 @@
       <c r="U8" s="6"/>
     </row>
     <row r="9" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="48"/>
+      <c r="D9" s="38"/>
       <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
@@ -1108,11 +1108,11 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="58" t="s">
+      <c r="K9" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="L9" s="56"/>
-      <c r="M9" s="64" t="s">
+      <c r="L9" s="34"/>
+      <c r="M9" s="32" t="s">
         <v>9</v>
       </c>
       <c r="N9" s="6"/>
@@ -1125,10 +1125,10 @@
       <c r="U9" s="6"/>
     </row>
     <row r="10" spans="2:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="46"/>
+      <c r="D10" s="48"/>
       <c r="E10" s="10" t="s">
         <v>9</v>
       </c>
@@ -1136,15 +1136,15 @@
       <c r="G10" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="51"/>
+      <c r="H10" s="27"/>
       <c r="I10" s="24" t="s">
         <v>7</v>
       </c>
       <c r="J10" s="6"/>
-      <c r="K10" s="59" t="s">
+      <c r="K10" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="57"/>
+      <c r="L10" s="50"/>
       <c r="M10" s="25" t="s">
         <v>9</v>
       </c>
@@ -1165,15 +1165,15 @@
       <c r="G11" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="52"/>
+      <c r="H11" s="28"/>
       <c r="I11" s="25" t="s">
         <v>7</v>
       </c>
       <c r="J11" s="6"/>
-      <c r="K11" s="33" t="s">
+      <c r="K11" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="L11" s="34"/>
+      <c r="L11" s="44"/>
       <c r="M11" s="12" t="s">
         <v>9</v>
       </c>
@@ -1194,15 +1194,15 @@
       <c r="G12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="52"/>
+      <c r="H12" s="28"/>
       <c r="I12" s="25" t="s">
         <v>7</v>
       </c>
       <c r="J12" s="6"/>
-      <c r="K12" s="33" t="s">
+      <c r="K12" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="34"/>
+      <c r="L12" s="44"/>
       <c r="M12" s="12" t="s">
         <v>9</v>
       </c>
@@ -1225,23 +1225,23 @@
       <c r="G13" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="53"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="26" t="s">
         <v>7</v>
       </c>
       <c r="J13" s="6"/>
-      <c r="K13" s="60" t="s">
+      <c r="K13" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="61"/>
-      <c r="M13" s="62" t="s">
+      <c r="L13" s="46"/>
+      <c r="M13" s="30" t="s">
         <v>9</v>
       </c>
       <c r="N13" s="6"/>
-      <c r="O13" s="44" t="s">
+      <c r="O13" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="P13" s="45"/>
+      <c r="P13" s="52"/>
       <c r="Q13" s="13" t="s">
         <v>9</v>
       </c>
@@ -1263,10 +1263,10 @@
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
-      <c r="O14" s="27" t="s">
+      <c r="O14" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="28"/>
+      <c r="P14" s="53"/>
       <c r="Q14" s="14" t="s">
         <v>9</v>
       </c>
@@ -1288,10 +1288,10 @@
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
-      <c r="O15" s="27" t="s">
+      <c r="O15" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="P15" s="28"/>
+      <c r="P15" s="53"/>
       <c r="Q15" s="14" t="s">
         <v>9</v>
       </c>
@@ -1313,10 +1313,10 @@
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
-      <c r="O16" s="27" t="s">
+      <c r="O16" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="P16" s="28"/>
+      <c r="P16" s="53"/>
       <c r="Q16" s="14" t="s">
         <v>10</v>
       </c>
@@ -1338,10 +1338,10 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="27" t="s">
+      <c r="O17" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="P17" s="28"/>
+      <c r="P17" s="53"/>
       <c r="Q17" s="14" t="s">
         <v>10</v>
       </c>
@@ -1363,10 +1363,10 @@
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
-      <c r="O18" s="27" t="s">
+      <c r="O18" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="P18" s="28"/>
+      <c r="P18" s="53"/>
       <c r="Q18" s="14" t="s">
         <v>10</v>
       </c>
@@ -1390,18 +1390,18 @@
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
-      <c r="O19" s="38" t="s">
+      <c r="O19" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="P19" s="41"/>
+      <c r="P19" s="55"/>
       <c r="Q19" s="15" t="s">
         <v>9</v>
       </c>
       <c r="R19" s="6"/>
-      <c r="S19" s="38" t="s">
+      <c r="S19" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="T19" s="41"/>
+      <c r="T19" s="55"/>
       <c r="U19" s="15" t="s">
         <v>9</v>
       </c>
@@ -1423,10 +1423,10 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
-      <c r="S20" s="42" t="s">
+      <c r="S20" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="T20" s="43"/>
+      <c r="T20" s="57"/>
       <c r="U20" s="14" t="s">
         <v>10</v>
       </c>
@@ -1448,10 +1448,10 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
-      <c r="S21" s="29" t="s">
+      <c r="S21" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="T21" s="37"/>
+      <c r="T21" s="59"/>
       <c r="U21" s="16" t="s">
         <v>9</v>
       </c>
@@ -1519,10 +1519,10 @@
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
       <c r="J24" s="6"/>
-      <c r="K24" s="31" t="s">
+      <c r="K24" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="L24" s="32"/>
+      <c r="L24" s="61"/>
       <c r="M24" s="11" t="s">
         <v>9</v>
       </c>
@@ -1531,10 +1531,10 @@
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
-      <c r="S24" s="38" t="s">
+      <c r="S24" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="T24" s="39"/>
+      <c r="T24" s="64"/>
       <c r="U24" s="15" t="s">
         <v>9</v>
       </c>
@@ -1548,10 +1548,10 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
-      <c r="K25" s="33" t="s">
+      <c r="K25" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="L25" s="34"/>
+      <c r="L25" s="44"/>
       <c r="M25" s="12" t="s">
         <v>9</v>
       </c>
@@ -1560,10 +1560,10 @@
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
-      <c r="S25" s="27" t="s">
+      <c r="S25" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="T25" s="40"/>
+      <c r="T25" s="42"/>
       <c r="U25" s="14" t="s">
         <v>9</v>
       </c>
@@ -1577,10 +1577,10 @@
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
-      <c r="K26" s="35" t="s">
+      <c r="K26" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="L26" s="36"/>
+      <c r="L26" s="63"/>
       <c r="M26" s="17" t="s">
         <v>9</v>
       </c>
@@ -1589,10 +1589,10 @@
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
-      <c r="S26" s="27" t="s">
+      <c r="S26" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="T26" s="28"/>
+      <c r="T26" s="53"/>
       <c r="U26" s="14" t="s">
         <v>10</v>
       </c>
@@ -1606,20 +1606,20 @@
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
-      <c r="K27" s="29" t="s">
+      <c r="K27" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="L27" s="37"/>
+      <c r="L27" s="59"/>
       <c r="M27" s="16"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
-      <c r="S27" s="27" t="s">
+      <c r="S27" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="T27" s="28"/>
+      <c r="T27" s="53"/>
       <c r="U27" s="14" t="s">
         <v>10</v>
       </c>
@@ -1641,44 +1641,21 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
-      <c r="S28" s="27" t="s">
+      <c r="S28" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="T28" s="28"/>
+      <c r="T28" s="53"/>
       <c r="U28" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="S29" s="29"/>
-      <c r="T29" s="30"/>
+      <c r="S29" s="58"/>
+      <c r="T29" s="60"/>
       <c r="U29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="S19:T19"/>
-    <mergeCell ref="S20:T20"/>
-    <mergeCell ref="S21:T21"/>
     <mergeCell ref="S28:T28"/>
     <mergeCell ref="S29:T29"/>
     <mergeCell ref="K24:L24"/>
@@ -1689,6 +1666,29 @@
     <mergeCell ref="S25:T25"/>
     <mergeCell ref="S26:T26"/>
     <mergeCell ref="S27:T27"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="S19:T19"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
patient report page done
</commit_message>
<xml_diff>
--- a/Database Model.xlsx
+++ b/Database Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KingSameulX/Desktop/Xcode/2020_05/P2P/v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E69824F-F69B-E445-894D-3F6070FDBD53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716A0E4E-D90F-A845-A93B-9000C59F8482}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" xr2:uid="{EDB24821-F2C5-425D-B33E-6AD2066199ED}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{EDB24821-F2C5-425D-B33E-6AD2066199ED}"/>
   </bookViews>
   <sheets>
     <sheet name="db" sheetId="1" r:id="rId1"/>
@@ -901,7 +901,7 @@
   <dimension ref="A1:AA29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>